<commit_message>
theme v2 mcd et a faire
</commit_message>
<xml_diff>
--- a/dotnet/documentation/a faire.xlsx
+++ b/dotnet/documentation/a faire.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="102">
   <si>
     <t>Membre</t>
   </si>
@@ -314,6 +314,96 @@
   </si>
   <si>
     <t>PREPARATION</t>
+  </si>
+  <si>
+    <t>FOND</t>
+  </si>
+  <si>
+    <t>Table fond</t>
+  </si>
+  <si>
+    <t>insertionTable</t>
+  </si>
+  <si>
+    <t>envoyeMail</t>
+  </si>
+  <si>
+    <t>view</t>
+  </si>
+  <si>
+    <t>insertion fond</t>
+  </si>
+  <si>
+    <t>PORTEFEUILLE CRYPTO</t>
+  </si>
+  <si>
+    <t>Table portefeuille_crypto</t>
+  </si>
+  <si>
+    <t>insertion table portefeuille_crypto</t>
+  </si>
+  <si>
+    <t>transformation crypto en fond</t>
+  </si>
+  <si>
+    <t>insertion table fond</t>
+  </si>
+  <si>
+    <t>calcul somme crypto *group id_crypto*</t>
+  </si>
+  <si>
+    <t>calcul somme fond</t>
+  </si>
+  <si>
+    <t>vente et achat crypto</t>
+  </si>
+  <si>
+    <t>affichage portefeuille et fond</t>
+  </si>
+  <si>
+    <t>COURS CRYPTO</t>
+  </si>
+  <si>
+    <t>Table crypto</t>
+  </si>
+  <si>
+    <t>Table cours_crypto</t>
+  </si>
+  <si>
+    <t>insertion table cours</t>
+  </si>
+  <si>
+    <t>select cours_crypto</t>
+  </si>
+  <si>
+    <t>calcul + ou - 10% derniere valeur *date NOW*</t>
+  </si>
+  <si>
+    <t>graph</t>
+  </si>
+  <si>
+    <t>*java *</t>
+  </si>
+  <si>
+    <r>
+      <t>entre et sortie</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> *form*</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">form </t>
+  </si>
+  <si>
+    <t>details portefeuille et fond de l utilisateur</t>
   </si>
 </sst>
 </file>
@@ -358,7 +448,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -426,16 +516,34 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -465,7 +573,27 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -770,10 +898,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1059,7 +1187,7 @@
         <v>23</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -1400,65 +1528,244 @@
       <c r="F44" s="2"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" s="13"/>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
+      <c r="A45" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" s="13"/>
-      <c r="B46" s="2"/>
+      <c r="A46" s="14"/>
+      <c r="B46" s="10"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" s="13"/>
-      <c r="B47" s="2"/>
+      <c r="A47" s="14"/>
+      <c r="B47" s="9" t="s">
+        <v>19</v>
+      </c>
       <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
+      <c r="D47" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" s="13"/>
-      <c r="B48" s="2"/>
+      <c r="A48" s="14"/>
+      <c r="B48" s="10"/>
       <c r="C48" s="2"/>
-      <c r="D48" s="2"/>
+      <c r="D48" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" s="2"/>
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
+      <c r="A49" s="15"/>
+      <c r="B49" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>99</v>
+      </c>
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" s="2"/>
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
+      <c r="A50" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>83</v>
+      </c>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="2"/>
-      <c r="B51" s="2"/>
+      <c r="A51" s="11"/>
+      <c r="B51" s="10"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
     </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" s="11"/>
+      <c r="B52" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D52" s="12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" s="11"/>
+      <c r="B53" s="18"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" s="11"/>
+      <c r="B54" s="18"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" s="11"/>
+      <c r="B55" s="18"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" s="11"/>
+      <c r="B56" s="19"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" s="11"/>
+      <c r="B57" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" s="10"/>
+      <c r="B58" s="10"/>
+      <c r="C58" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
+      <c r="F59" s="2"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" s="11"/>
+      <c r="B60" s="10"/>
+      <c r="C60" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2"/>
+      <c r="F60" s="2"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61" s="11"/>
+      <c r="B61" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E61" s="2"/>
+      <c r="F61" s="2"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62" s="11"/>
+      <c r="B62" s="11"/>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E62" s="2"/>
+      <c r="F62" s="2"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63" s="11"/>
+      <c r="B63" s="10"/>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E63" s="2"/>
+      <c r="F63" s="2"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" s="10"/>
+      <c r="B64" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="26">
+    <mergeCell ref="A50:A58"/>
+    <mergeCell ref="A59:A64"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="B52:B56"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="B59:B60"/>
+    <mergeCell ref="B61:B63"/>
     <mergeCell ref="B9:B13"/>
     <mergeCell ref="A9:A13"/>
+    <mergeCell ref="A45:A49"/>
     <mergeCell ref="C37:C41"/>
     <mergeCell ref="B35:B36"/>
     <mergeCell ref="A14:A22"/>

</xml_diff>